<commit_message>
Add invalid test cases in test_read_data.py
</commit_message>
<xml_diff>
--- a/integration_tests/resources/data.xlsx
+++ b/integration_tests/resources/data.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\saroa\repos\eddington\integration_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9005A54C-2DAF-4D7C-943C-E23619E89096}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68447A91-1EA5-4E04-87D7-A23C7FF3587A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{BD0826E8-52E5-4AE6-8F79-D7A0AF58B4B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{BD0826E8-52E5-4AE6-8F79-D7A0AF58B4B6}"/>
   </bookViews>
   <sheets>
     <sheet name="data1" sheetId="1" r:id="rId1"/>
+    <sheet name="invalid_data1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
   <si>
     <t>a</t>
   </si>
@@ -405,8 +406,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0070D683-CA49-4787-841B-E8183B5BC6E9}">
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -574,4 +575,176 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9811A672-EC6E-4968-9B33-1801508244B0}">
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0.5</v>
+      </c>
+      <c r="C2">
+        <v>16</v>
+      </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>100</v>
+      </c>
+      <c r="F2">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>29</v>
+      </c>
+      <c r="D3">
+        <v>1.3</v>
+      </c>
+      <c r="E3">
+        <v>401</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>30</v>
+      </c>
+      <c r="B4">
+        <v>1.2</v>
+      </c>
+      <c r="C4">
+        <v>47</v>
+      </c>
+      <c r="D4">
+        <v>0.8</v>
+      </c>
+      <c r="E4">
+        <v>910</v>
+      </c>
+      <c r="F4">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>40</v>
+      </c>
+      <c r="B5">
+        <v>0.3</v>
+      </c>
+      <c r="C5">
+        <v>56</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="E5">
+        <v>1559</v>
+      </c>
+      <c r="F5">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>50</v>
+      </c>
+      <c r="B6">
+        <v>0.4</v>
+      </c>
+      <c r="C6">
+        <v>70</v>
+      </c>
+      <c r="E6">
+        <v>2480</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>60</v>
+      </c>
+      <c r="B7">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C7">
+        <v>92</v>
+      </c>
+      <c r="D7">
+        <v>0.2</v>
+      </c>
+      <c r="E7">
+        <v>3623</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>70</v>
+      </c>
+      <c r="B8">
+        <v>1.3</v>
+      </c>
+      <c r="C8">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>2</v>
+      </c>
+      <c r="E8">
+        <v>4910</v>
+      </c>
+      <c r="F8">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>